<commit_message>
created spreadsheet and script to auto generate html
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekklc/Desktop/HTML/kate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9936DD9C-B866-E540-9501-DC7AF97742D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1DE34E-A21E-2F4A-8CBD-B9AD9CA739FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27560" windowHeight="17040" xr2:uid="{C541567E-6F35-2746-9218-E04ED4A33C37}"/>
   </bookViews>
@@ -34,19 +34,241 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>title1</t>
-  </si>
-  <si>
-    <t>type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="72">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Keychron K3 Ultra-slim Wireless Mechanical Keyboard (Version 2)</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>note1</t>
+  </si>
+  <si>
+    <t>note2</t>
+  </si>
+  <si>
+    <t>note3</t>
+  </si>
+  <si>
+    <t>menu_1_button</t>
+  </si>
+  <si>
+    <t>Specifications</t>
+  </si>
+  <si>
+    <t>Connectivity</t>
+  </si>
+  <si>
+    <t>main_title</t>
+  </si>
+  <si>
+    <t>Physical Unit</t>
+  </si>
+  <si>
+    <t>Package Content</t>
+  </si>
+  <si>
+    <t>Number of Keys: 84 keys</t>
+  </si>
+  <si>
+    <t>Layout: ANSI</t>
+  </si>
+  <si>
+    <t>Version: Gateron</t>
+  </si>
+  <si>
+    <t>Switches: Low profile Gateron mechanical</t>
+  </si>
+  <si>
+    <t>Number of Multimedia Keys: 12</t>
+  </si>
+  <si>
+    <t>menu_1_body_row_1</t>
+  </si>
+  <si>
+    <t>Frame Material: ABS+Aluminum frame</t>
+  </si>
+  <si>
+    <t>Keycap Material: ABS</t>
+  </si>
+  <si>
+    <t>Backlit: White backlit</t>
+  </si>
+  <si>
+    <t>Backlit Types: 18</t>
+  </si>
+  <si>
+    <t>System: Windows/Android/Mac/iOS</t>
+  </si>
+  <si>
+    <t>Battery: 1550mAh Rechargeable li-polymer battery</t>
+  </si>
+  <si>
+    <t>BT Working Time (Single LED): Up to 34 hours (Lab test result may vary by actual use)</t>
+  </si>
+  <si>
+    <t>Connection: Bluetooth and Type-C cable</t>
+  </si>
+  <si>
+    <t>Bluetooth version: 5.1</t>
+  </si>
+  <si>
+    <t>Bluetooth Device Name: Keychron K3</t>
+  </si>
+  <si>
+    <t>Compatible System: macOS/Windows</t>
+  </si>
+  <si>
+    <t>Height incl. keycap (front) 22mm</t>
+  </si>
+  <si>
+    <t>Height incl. keycap (rear) 17mm</t>
+  </si>
+  <si>
+    <t>DimeWeight: About 396g / 0.87lbsnsion</t>
+  </si>
+  <si>
+    <t>Operating Environment: -10 to 50 °C (Celcius degrees)</t>
+  </si>
+  <si>
+    <t>1 x Keyboard</t>
+  </si>
+  <si>
+    <t>1 x Keycap Puller</t>
+  </si>
+  <si>
+    <t>1 x Dust Cover</t>
+  </si>
+  <si>
+    <t>1 x User Manual</t>
+  </si>
+  <si>
+    <t>Dimension: 306 x 116mm</t>
+  </si>
+  <si>
+    <t>top_title</t>
+  </si>
+  <si>
+    <t>Keychron K3v2 Low-Profile Bluetooth Keyboard Wireless/Wired Gateron 84 Key Ultra</t>
+  </si>
+  <si>
+    <t>body_img_1</t>
+  </si>
+  <si>
+    <t>https://mastex.com.au/wp-content/uploads/2021/08/K3A.jpg</t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>The newly arrived &lt;strong&gt;Keychron K3&lt;/strong&gt; Keyboard comes with keycaps for both Windows and Mac users. It is an Ultra-slim wireless mechanical keyboard that provides you with smooth and comfortable typing experience.</t>
+  </si>
+  <si>
+    <t>Designed by our ergonomics professionals. This keyboard incorporates world's first &lt;strong&gt;hot-swappable low profile Optical switches&lt;/strong&gt; to customize per-key typing experience with ease, together with all signature Keychron features.</t>
+  </si>
+  <si>
+    <t>Wireless and Wired</t>
+  </si>
+  <si>
+    <t>https://mastex.com.au/wp-content/uploads/2022/02/double-shot-keycap-lightgrey.jpg"</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Keychron K3&lt;/strong&gt; keyboard connects via Type-C or Bluetooth(Broadcom Bluetooth 5.1) allowing up to 3 devices, and switching in between has been made super easily. Featuring Bluetooth 5.1 chipset, the keyboard offers flawless connectivity whether you are working at home or the office while connected with your smartphone, laptop or iPad.</t>
+  </si>
+  <si>
+    <t>Ultra Slim</t>
+  </si>
+  <si>
+    <t>https://mastex.com.au/wp-content/uploads/2022/02/oem_Unicorn.jpg</t>
+  </si>
+  <si>
+    <t>The redesigned low profile switch is 40% slimmer than conventional switches. Together with the streamlined aluminum body makes the K3 one of the thinnest and lightweight wireless mechanical keyboards in the world.</t>
+  </si>
+  <si>
+    <t>Suitable for All Devices</t>
+  </si>
+  <si>
+    <t>https://mastex.com.au/wp-content/uploads/2022/02/double-shot-keycap-lightgrey.jpg</t>
+  </si>
+  <si>
+    <t>Compatible with both macOS and Windows. Keychron is one of only a few in the market that comes with a Mac multimedia keys layout for Mac enthusiasts. For Linux users, we also have a dedicated user group to help with the experience.</t>
+  </si>
+  <si>
+    <t>Two-Level Adjustment</t>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0059/0630/1017/t/5/assets/pf-6664eb64--KeychronK3keyboardlayout1000.png?v=1602660593</t>
+  </si>
+  <si>
+    <t>Two level adjustable rubber feet makes the new K3 more comfortable to type on.</t>
+  </si>
+  <si>
+    <t>Mechanical Switch</t>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0059/0630/1017/t/5/assets/pf-d698a4c8--k3version2adjustablefeet-Edited?v=1622451026</t>
+  </si>
+  <si>
+    <t>Durable low profile Gateron Mechanical switch with a 50 million keystroke lifespan to provide an unrivaled tactile responsiveness.</t>
+  </si>
+  <si>
+    <t>Alternative Keycaps</t>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0059/0630/1017/t/5/assets/pf-3d7405f5--KeychronK3LowProfileGateronSwitchspecs.jpeg?v=1626750223</t>
+  </si>
+  <si>
+    <t>75% LAYOUT</t>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0059/0630/1017/t/5/assets/pf-f109ef5d--KeychronK3ultraslimwirelessmechanicalkeyboardmacwindowsiOSandroidKeychronOpticalGateronmechanicalswitchredbluebrownkeycapcompareRoccatVulcan120AimoCherrylowprofilekeycap.jpeg?v=1602593873</t>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0059/0630/1017/t/5/assets/pf-d006a42c--KeychronK3ultraslimHotswappablewirelessBluetoothmechanicalkeyboardMacWindowsiOSAndroidKeychronlowprofileOpticalGateronlowprofilemechanicalswitchredbluebrownwhiteblackorangedesktoplayout.jpg?v=1602595361</t>
+  </si>
+  <si>
+    <t>Crafted for productivity, the K3's 75% layout is a compact version of tenkeyless layout. It allows users access to all the essential multimedia and function keys, but with a smaller footprint.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Taking more than a year of dedicated development and testing, we are bring users with the MX-styled stem on both the low profile switches for K3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;strong&gt;PLUS&lt;/strong&gt; the stabilizers on the big keys like the space bar, left Shift, backspace and Enter key.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0059/0630/1017/t/5/assets/pf-481ce134--KeychronK3ultraslimcompactHotswappablewirelessmechanicalkeyboardMacWindowsiOSAndroidlowprofileKeychronOpticalandGateronmechanicalswitchredbluebrownwhiteblackorange.png?v=1602585488</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>body_section_item_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,13 +276,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,13 +321,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,25 +656,750 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F90DBF-9F09-4D46-B4C5-F3284942CD03}">
-  <dimension ref="D3:D4"/>
+  <dimension ref="C1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
+    <row r="1" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>0</v>
+    <row r="5" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="C44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="C45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="1">
+        <v>3</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="C47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="1">
+        <v>4</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="C48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="1">
+        <v>4</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="1">
+        <v>5</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="C50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="C51" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" s="1">
+        <v>5</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C52" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="1">
+        <v>6</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="C53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="1">
+        <v>6</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="C54" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54" s="1">
+        <v>6</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="1">
+        <v>7</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="C56" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" s="1">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" s="1">
+        <v>7</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E58" s="1">
+        <v>8</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="C59" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" s="1">
+        <v>8</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="C60" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="1">
+        <v>8</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="C61" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E61" s="1">
+        <v>8</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D37" r:id="rId1" xr:uid="{9BE1CA12-7E5B-CE4D-8300-A85E29D18644}"/>
+    <hyperlink ref="D47" r:id="rId2" xr:uid="{97E7D25C-C4C5-CD4A-B835-92859D11ED28}"/>
+    <hyperlink ref="D56" r:id="rId3" xr:uid="{671DF6B5-4914-E147-B78B-DCDA6FF5BA82}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>